<commit_message>
WIP LaTeX and code mark-up
Doing code final touches and finishing write-up in LaTeX.
</commit_message>
<xml_diff>
--- a/Assignment 2/figures/Results.xlsx
+++ b/Assignment 2/figures/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://landfallnavigation-my.sharepoint.com/personal/connor_landfallnavigation_onmicrosoft_com/Documents/Documents/School/3a Junior Sem 1/Algorithm Analysis &amp; Design - Cmpt 435/Algorithms/Assignment 2/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="260" documentId="11_F25DC773A252ABDACC1048B2D99B40945ADE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CBBDE86-95B0-4572-8F5B-4E98C3A00E7E}"/>
+  <xr:revisionPtr revIDLastSave="269" documentId="11_F25DC773A252ABDACC1048B2D99B40945ADE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F2AC661-567C-4239-BDDD-C6076992626A}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,26 +92,44 @@
     <t>Hshsearch expected:</t>
   </si>
   <si>
-    <t>O(log(2) (n)) ~</t>
-  </si>
-  <si>
-    <t>O(n/250) ~</t>
-  </si>
-  <si>
-    <t>O(n/2) ~</t>
-  </si>
-  <si>
     <t>Better than expected?</t>
   </si>
   <si>
     <t>Search vector size:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>Θ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n/2) ~</t>
+    </r>
+  </si>
+  <si>
+    <t>Θ(log(2) (n)) ~</t>
+  </si>
+  <si>
+    <t>Θ(n/250) ~</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +150,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -187,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -204,6 +228,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -228,11 +253,15 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C9C7D21-28B7-4BEA-89D6-54F31B451A37}" name="Table1" displayName="Table1" ref="G2:I5" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{008A4DDE-F272-40A8-9728-CB6076D2E3F8}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{1FB0B6F8-4EC5-4205-BCBF-22281114BED5}" name="Column2" headerRowDxfId="0" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{1FB0B6F8-4EC5-4205-BCBF-22281114BED5}" name="Column2" headerRowDxfId="1" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{08DFD634-87A5-48F3-85C6-0603D52A104B}" name="Column3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -505,7 +534,7 @@
   <dimension ref="B1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -526,7 +555,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.35">
@@ -537,7 +566,7 @@
         <v>315.88</v>
       </c>
       <c r="D2" s="11" t="str">
-        <f>IF(C2&lt;$I$2,"True","False")</f>
+        <f t="shared" ref="D2:D12" si="0">IF(C2&lt;$I$2,"True","False")</f>
         <v>True</v>
       </c>
       <c r="G2" t="s">
@@ -559,14 +588,14 @@
         <v>364.76</v>
       </c>
       <c r="D3" s="9" t="str">
-        <f>IF(C3&lt;$I$2,"True","False")</f>
+        <f t="shared" si="0"/>
         <v>False</v>
       </c>
       <c r="G3" t="s">
         <v>16</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I3" s="1">
         <f xml:space="preserve"> LOG(H5, 2)</f>
@@ -581,14 +610,14 @@
         <v>361.38</v>
       </c>
       <c r="D4" s="10" t="str">
-        <f>IF(C4&lt;$I$2,"True","False")</f>
+        <f t="shared" si="0"/>
         <v>False</v>
       </c>
       <c r="G4" t="s">
         <v>17</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I4" s="1">
         <f>(H5/250)</f>
@@ -603,11 +632,11 @@
         <v>360.88</v>
       </c>
       <c r="D5" s="9" t="str">
-        <f>IF(C5&lt;$I$2,"True","False")</f>
+        <f t="shared" si="0"/>
         <v>False</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H5">
         <v>666</v>
@@ -621,7 +650,7 @@
         <v>359.14</v>
       </c>
       <c r="D6" s="10" t="str">
-        <f>IF(C6&lt;$I$2,"True","False")</f>
+        <f t="shared" si="0"/>
         <v>False</v>
       </c>
     </row>
@@ -633,7 +662,7 @@
         <v>378.05</v>
       </c>
       <c r="D7" s="9" t="str">
-        <f>IF(C7&lt;$I$2,"True","False")</f>
+        <f t="shared" si="0"/>
         <v>False</v>
       </c>
     </row>
@@ -645,7 +674,7 @@
         <v>340.86</v>
       </c>
       <c r="D8" s="10" t="str">
-        <f>IF(C8&lt;$I$2,"True","False")</f>
+        <f t="shared" si="0"/>
         <v>False</v>
       </c>
     </row>
@@ -657,7 +686,7 @@
         <v>329.12</v>
       </c>
       <c r="D9" s="12" t="str">
-        <f>IF(C9&lt;$I$2,"True","False")</f>
+        <f t="shared" si="0"/>
         <v>True</v>
       </c>
     </row>
@@ -669,7 +698,7 @@
         <v>403.07</v>
       </c>
       <c r="D10" s="10" t="str">
-        <f>IF(C10&lt;$I$2,"True","False")</f>
+        <f t="shared" si="0"/>
         <v>False</v>
       </c>
     </row>
@@ -677,11 +706,11 @@
       <c r="B11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="14">
         <v>330.6</v>
       </c>
       <c r="D11" s="12" t="str">
-        <f>IF(C11&lt;$I$2,"True","False")</f>
+        <f t="shared" si="0"/>
         <v>True</v>
       </c>
     </row>
@@ -689,12 +718,12 @@
       <c r="B12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <f xml:space="preserve"> SUM(C2:C11)/10</f>
         <v>354.37400000000002</v>
       </c>
       <c r="D12" s="10" t="str">
-        <f>IF(C12&lt;$I$2,"True","False")</f>
+        <f t="shared" si="0"/>
         <v>False</v>
       </c>
     </row>
@@ -706,7 +735,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.35">
@@ -717,7 +746,7 @@
         <v>8.3800000000000008</v>
       </c>
       <c r="D15" s="11" t="str">
-        <f>IF(C15&lt;$I$3,"True","False")</f>
+        <f t="shared" ref="D15:D25" si="1">IF(C15&lt;$I$3,"True","False")</f>
         <v>True</v>
       </c>
     </row>
@@ -729,7 +758,7 @@
         <v>8.7100000000000009</v>
       </c>
       <c r="D16" s="12" t="str">
-        <f>IF(C16&lt;$I$3,"True","False")</f>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
     </row>
@@ -741,7 +770,7 @@
         <v>8.43</v>
       </c>
       <c r="D17" s="11" t="str">
-        <f>IF(C17&lt;$I$3,"True","False")</f>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
     </row>
@@ -753,7 +782,7 @@
         <v>8.36</v>
       </c>
       <c r="D18" s="12" t="str">
-        <f>IF(C18&lt;$I$3,"True","False")</f>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
     </row>
@@ -765,7 +794,7 @@
         <v>8.17</v>
       </c>
       <c r="D19" s="11" t="str">
-        <f>IF(C19&lt;$I$3,"True","False")</f>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
     </row>
@@ -773,11 +802,11 @@
       <c r="B20" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="14">
         <v>8.4</v>
       </c>
       <c r="D20" s="12" t="str">
-        <f>IF(C20&lt;$I$3,"True","False")</f>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
     </row>
@@ -789,7 +818,7 @@
         <v>8.81</v>
       </c>
       <c r="D21" s="11" t="str">
-        <f>IF(C21&lt;$I$3,"True","False")</f>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
     </row>
@@ -801,7 +830,7 @@
         <v>8.81</v>
       </c>
       <c r="D22" s="12" t="str">
-        <f>IF(C22&lt;$I$3,"True","False")</f>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
     </row>
@@ -813,7 +842,7 @@
         <v>8.67</v>
       </c>
       <c r="D23" s="11" t="str">
-        <f>IF(C23&lt;$I$3,"True","False")</f>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
     </row>
@@ -825,7 +854,7 @@
         <v>8.31</v>
       </c>
       <c r="D24" s="12" t="str">
-        <f>IF(C24&lt;$I$3,"True","False")</f>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
     </row>
@@ -833,12 +862,12 @@
       <c r="B25" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="6">
         <f xml:space="preserve"> SUM(C15:C24)/10</f>
         <v>8.5050000000000008</v>
       </c>
       <c r="D25" s="11" t="str">
-        <f>IF(C25&lt;$I$3,"True","False")</f>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
     </row>
@@ -850,7 +879,7 @@
         <v>13</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.35">
@@ -861,7 +890,7 @@
         <v>1.5</v>
       </c>
       <c r="D28" s="11" t="str">
-        <f>IF(C28&lt;$I$4,"True","False")</f>
+        <f t="shared" ref="D28:D38" si="2">IF(C28&lt;$I$4,"True","False")</f>
         <v>True</v>
       </c>
     </row>
@@ -873,7 +902,7 @@
         <v>2.79</v>
       </c>
       <c r="D29" s="9" t="str">
-        <f>IF(C29&lt;$I$4,"True","False")</f>
+        <f t="shared" si="2"/>
         <v>False</v>
       </c>
     </row>
@@ -885,7 +914,7 @@
         <v>3.12</v>
       </c>
       <c r="D30" s="10" t="str">
-        <f>IF(C30&lt;$I$4,"True","False")</f>
+        <f t="shared" si="2"/>
         <v>False</v>
       </c>
     </row>
@@ -897,7 +926,7 @@
         <v>3.19</v>
       </c>
       <c r="D31" s="9" t="str">
-        <f>IF(C31&lt;$I$4,"True","False")</f>
+        <f t="shared" si="2"/>
         <v>False</v>
       </c>
     </row>
@@ -909,7 +938,7 @@
         <v>1.19</v>
       </c>
       <c r="D32" s="11" t="str">
-        <f>IF(C32&lt;$I$4,"True","False")</f>
+        <f t="shared" si="2"/>
         <v>True</v>
       </c>
     </row>
@@ -921,7 +950,7 @@
         <v>1.64</v>
       </c>
       <c r="D33" s="12" t="str">
-        <f>IF(C33&lt;$I$4,"True","False")</f>
+        <f t="shared" si="2"/>
         <v>True</v>
       </c>
     </row>
@@ -933,7 +962,7 @@
         <v>1.95</v>
       </c>
       <c r="D34" s="11" t="str">
-        <f>IF(C34&lt;$I$4,"True","False")</f>
+        <f t="shared" si="2"/>
         <v>True</v>
       </c>
     </row>
@@ -945,7 +974,7 @@
         <v>2.29</v>
       </c>
       <c r="D35" s="12" t="str">
-        <f>IF(C35&lt;$I$4,"True","False")</f>
+        <f t="shared" si="2"/>
         <v>True</v>
       </c>
     </row>
@@ -957,7 +986,7 @@
         <v>2.98</v>
       </c>
       <c r="D36" s="10" t="str">
-        <f>IF(C36&lt;$I$4,"True","False")</f>
+        <f t="shared" si="2"/>
         <v>False</v>
       </c>
     </row>
@@ -969,7 +998,7 @@
         <v>3.05</v>
       </c>
       <c r="D37" s="9" t="str">
-        <f>IF(C37&lt;$I$4,"True","False")</f>
+        <f t="shared" si="2"/>
         <v>False</v>
       </c>
     </row>
@@ -982,7 +1011,7 @@
         <v>2.37</v>
       </c>
       <c r="D38" s="11" t="str">
-        <f>IF(C38&lt;$I$4,"True","False")</f>
+        <f t="shared" si="2"/>
         <v>True</v>
       </c>
     </row>

</xml_diff>